<commit_message>
Add learning and test data excels
</commit_message>
<xml_diff>
--- a/data/test_data.xlsx
+++ b/data/test_data.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raynor\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7890" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="69">
   <si>
     <t>Message</t>
   </si>
@@ -328,6 +333,9 @@
 On Tue, Apr 14, 2015 at 5:14 PM, Jordan Donald &lt;jordan.donald@mail.hsa.net&gt; wrote:
 Works for me too!
 On Tue, Apr 14, 2015 at 5:10 PM, Diana Im &lt;diana.i</t>
+  </si>
+  <si>
+    <t>Event</t>
   </si>
 </sst>
 </file>
@@ -377,6 +385,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -702,20 +718,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="3" max="3" width="24.83203125" customWidth="1"/>
     <col min="4" max="4" width="218.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -728,8 +744,11 @@
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="409">
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>42109.899259259262</v>
       </c>
@@ -743,7 +762,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="409">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>42109.896458333336</v>
       </c>
@@ -757,7 +776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="409">
+    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>42109.8909375</v>
       </c>
@@ -771,7 +790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="105">
+    <row r="5" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>42109.888090277775</v>
       </c>
@@ -785,7 +804,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="90">
+    <row r="6" spans="1:5" ht="93" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>42109.834027777775</v>
       </c>
@@ -799,7 +818,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="165">
+    <row r="7" spans="1:5" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>42109.824016203704</v>
       </c>
@@ -813,7 +832,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="90">
+    <row r="8" spans="1:5" ht="93" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>42109.710509259261</v>
       </c>
@@ -827,7 +846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="90">
+    <row r="9" spans="1:5" ht="93" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>42109.709780092591</v>
       </c>
@@ -841,7 +860,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="195">
+    <row r="10" spans="1:5" ht="201.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>42109.665300925924</v>
       </c>
@@ -855,7 +874,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="105">
+    <row r="11" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>42109.656030092592</v>
       </c>
@@ -869,7 +888,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="90">
+    <row r="12" spans="1:5" ht="93" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>42109.655659722222</v>
       </c>
@@ -883,7 +902,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="75">
+    <row r="13" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>42109.65111111111</v>
       </c>
@@ -897,7 +916,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="105">
+    <row r="14" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>42109.648622685185</v>
       </c>
@@ -911,7 +930,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="150">
+    <row r="15" spans="1:5" ht="155" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>42109.644375000003</v>
       </c>
@@ -925,7 +944,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="105">
+    <row r="16" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>42109.642754629633</v>
       </c>
@@ -939,7 +958,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="90">
+    <row r="17" spans="1:4" ht="93" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>42109.638310185182</v>
       </c>
@@ -953,7 +972,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="409">
+    <row r="18" spans="1:4" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>42109.637303240743</v>
       </c>
@@ -967,7 +986,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="60">
+    <row r="19" spans="1:4" ht="62" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>42109.630416666667</v>
       </c>
@@ -981,7 +1000,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="180">
+    <row r="20" spans="1:4" ht="186" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>42109.629652777781</v>
       </c>
@@ -995,7 +1014,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="150">
+    <row r="21" spans="1:4" ht="155" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>42109.627939814818</v>
       </c>
@@ -1009,7 +1028,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="75">
+    <row r="22" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>42109.62740740741</v>
       </c>
@@ -1023,7 +1042,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="105">
+    <row r="23" spans="1:4" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>42109.626701388886</v>
       </c>
@@ -1037,7 +1056,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="75">
+    <row r="24" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>42109.374386574076</v>
       </c>
@@ -1051,7 +1070,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="165">
+    <row r="25" spans="1:4" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>42109.359803240739</v>
       </c>

</xml_diff>

<commit_message>
All shit works, but ugly and simple
</commit_message>
<xml_diff>
--- a/data/test_data.xlsx
+++ b/data/test_data.xlsx
@@ -720,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="40" zoomScaleNormal="40" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -761,6 +761,9 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
@@ -775,6 +778,9 @@
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
@@ -789,6 +795,9 @@
       <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
@@ -803,6 +812,9 @@
       <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="93" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
@@ -817,6 +829,9 @@
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
@@ -831,6 +846,9 @@
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="93" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
@@ -845,6 +863,9 @@
       <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="93" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
@@ -859,6 +880,9 @@
       <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="201.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
@@ -873,6 +897,9 @@
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
@@ -887,6 +914,9 @@
       <c r="D11" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="93" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
@@ -901,6 +931,9 @@
       <c r="D12" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
@@ -915,6 +948,9 @@
       <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
@@ -929,6 +965,9 @@
       <c r="D14" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="155" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
@@ -943,6 +982,9 @@
       <c r="D15" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
@@ -957,8 +999,11 @@
       <c r="D16" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="93" x14ac:dyDescent="0.35">
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="93" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>42109.638310185182</v>
       </c>
@@ -971,8 +1016,11 @@
       <c r="D17" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>42109.637303240743</v>
       </c>
@@ -985,8 +1033,11 @@
       <c r="D18" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="62" x14ac:dyDescent="0.35">
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="62" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>42109.630416666667</v>
       </c>
@@ -999,8 +1050,11 @@
       <c r="D19" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="186" x14ac:dyDescent="0.35">
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="186" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>42109.629652777781</v>
       </c>
@@ -1013,8 +1067,11 @@
       <c r="D20" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="155" x14ac:dyDescent="0.35">
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="155" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>42109.627939814818</v>
       </c>
@@ -1027,8 +1084,11 @@
       <c r="D21" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>42109.62740740741</v>
       </c>
@@ -1041,8 +1101,11 @@
       <c r="D22" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>42109.626701388886</v>
       </c>
@@ -1055,8 +1118,11 @@
       <c r="D23" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>42109.374386574076</v>
       </c>
@@ -1069,8 +1135,11 @@
       <c r="D24" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="170.5" x14ac:dyDescent="0.35">
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>42109.359803240739</v>
       </c>
@@ -1082,6 +1151,9 @@
       </c>
       <c r="D25" s="1" t="s">
         <v>67</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>